<commit_message>
Generate fraud detection report with both fraud categorization and metadata
</commit_message>
<xml_diff>
--- a/Fraud_Detection_Report.xlsx
+++ b/Fraud_Detection_Report.xlsx
@@ -29,7 +29,7 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -54,6 +54,12 @@
         <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFFF"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -73,7 +79,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -81,6 +87,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -446,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,7 +522,7 @@
         <v>431.4</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>68.60000000000002</v>
+        <v>68.59999999999999</v>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
@@ -566,67 +573,143 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Spirometry (procedure)</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>15000</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>7786.47</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>7213.53</v>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>Fraud</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>Standard pregnancy test</t>
         </is>
       </c>
-      <c r="B6" s="3" t="n">
+      <c r="B7" s="3" t="n">
         <v>5700</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C7" s="3" t="n">
         <v>5656.6</v>
       </c>
-      <c r="D6" s="3" t="n">
-        <v>43.39999999999964</v>
-      </c>
-      <c r="E6" s="3" t="inlineStr">
+      <c r="D7" s="3" t="n">
+        <v>43.4</v>
+      </c>
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>Legitimate</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Throat culture (procedure)</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>2300</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>2020.43</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>279.57</v>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Upper arm X-ray</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>431.4</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>1068.6</v>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Risk</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>Prostatectomy</t>
         </is>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B10" s="4" t="n">
         <v>10500</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C10" s="4" t="n">
         <v>6142.64</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D10" s="4" t="n">
         <v>4357.36</v>
       </c>
-      <c r="E7" s="4" t="inlineStr">
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>Fraud</t>
         </is>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+    <row r="11">
+      <c r="A11" s="3" t="inlineStr">
         <is>
           <t>Intubation</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B11" s="3" t="n">
         <v>500</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C11" s="3" t="n">
         <v>440.38</v>
       </c>
-      <c r="D8" s="3" t="n">
+      <c r="D11" s="3" t="n">
         <v>59.62</v>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t>Legitimate</t>
         </is>
       </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Total Invoice Amount</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>66433.10000000001</v>
+      </c>
+      <c r="C12" s="5" t="inlineStr"/>
+      <c r="D12" s="5" t="inlineStr"/>
+      <c r="E12" s="5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>